<commit_message>
Entradas x saidas:  -CC
</commit_message>
<xml_diff>
--- a/assets/cost_sheet.xlsx
+++ b/assets/cost_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56C9449150E6BC49/Documentos/FEARP/Intercambio/spendure_app/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1519" documentId="8_{697955BF-7644-43E6-B102-A5718628249A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16182895-BB9A-4AF5-9E92-66CD4B8E29D4}"/>
+  <xr:revisionPtr revIDLastSave="1521" documentId="8_{697955BF-7644-43E6-B102-A5718628249A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B76592F7-4DA2-42B5-88CA-9E2FB9A7D61B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3A902579-E7D0-4425-859E-D7B710BECD9D}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table!$A$1:$I$238</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table!$A$1:$I$237</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="208">
   <si>
     <t>Data</t>
   </si>
@@ -786,6 +786,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1105,10 +1109,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D03841-840F-48EF-840B-36FDA2E59E7D}">
-  <dimension ref="A1:I646"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I645"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="B239" sqref="B239"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1152,7 +1157,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45657</v>
       </c>
@@ -1177,7 +1182,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45659</v>
       </c>
@@ -1202,7 +1207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45659</v>
       </c>
@@ -1227,7 +1232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45659</v>
       </c>
@@ -1252,7 +1257,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45659</v>
       </c>
@@ -1277,7 +1282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45659</v>
       </c>
@@ -1302,7 +1307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45660</v>
       </c>
@@ -1327,7 +1332,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45660</v>
       </c>
@@ -1352,7 +1357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45660</v>
       </c>
@@ -1377,7 +1382,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45660</v>
       </c>
@@ -1402,7 +1407,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>45661</v>
       </c>
@@ -1427,7 +1432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>45661</v>
       </c>
@@ -1452,7 +1457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>45662</v>
       </c>
@@ -1481,7 +1486,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>45662</v>
       </c>
@@ -1506,7 +1511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>45663</v>
       </c>
@@ -1531,7 +1536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>45663</v>
       </c>
@@ -1556,7 +1561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>45663</v>
       </c>
@@ -1581,7 +1586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>45664</v>
       </c>
@@ -1606,7 +1611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>45664</v>
       </c>
@@ -1631,7 +1636,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>45664</v>
       </c>
@@ -1656,7 +1661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>45666</v>
       </c>
@@ -1679,7 +1684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45666</v>
       </c>
@@ -1704,7 +1709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>45667</v>
       </c>
@@ -1729,7 +1734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>45667</v>
       </c>
@@ -1754,7 +1759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>45668</v>
       </c>
@@ -1779,7 +1784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>45668</v>
       </c>
@@ -1804,7 +1809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>45668</v>
       </c>
@@ -1829,7 +1834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>45668</v>
       </c>
@@ -1854,7 +1859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45669</v>
       </c>
@@ -1879,7 +1884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>45669</v>
       </c>
@@ -1904,7 +1909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>45669</v>
       </c>
@@ -1929,7 +1934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>45670</v>
       </c>
@@ -1954,7 +1959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>45670</v>
       </c>
@@ -1979,7 +1984,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>45670</v>
       </c>
@@ -2054,7 +2059,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>45674</v>
       </c>
@@ -2079,7 +2084,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>45676</v>
       </c>
@@ -2104,7 +2109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>45676</v>
       </c>
@@ -2129,7 +2134,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>45677</v>
       </c>
@@ -2158,7 +2163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>45677</v>
       </c>
@@ -2183,7 +2188,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>45677</v>
       </c>
@@ -2208,7 +2213,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>45678</v>
       </c>
@@ -2233,7 +2238,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>45678</v>
       </c>
@@ -2258,7 +2263,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45678</v>
       </c>
@@ -2283,7 +2288,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45679</v>
       </c>
@@ -2308,7 +2313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>45680</v>
       </c>
@@ -2333,7 +2338,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>45681</v>
       </c>
@@ -2358,7 +2363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>45681</v>
       </c>
@@ -2383,7 +2388,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>45681</v>
       </c>
@@ -2408,7 +2413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>45681</v>
       </c>
@@ -2433,7 +2438,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>45682</v>
       </c>
@@ -2458,7 +2463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>45683</v>
       </c>
@@ -2483,7 +2488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>45684</v>
       </c>
@@ -2508,7 +2513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>45684</v>
       </c>
@@ -2533,7 +2538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>45685</v>
       </c>
@@ -2558,7 +2563,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>45687</v>
       </c>
@@ -2583,7 +2588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>45687</v>
       </c>
@@ -2608,7 +2613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>45687</v>
       </c>
@@ -2633,7 +2638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>45688</v>
       </c>
@@ -2658,7 +2663,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>45688</v>
       </c>
@@ -2683,7 +2688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>45688</v>
       </c>
@@ -2708,7 +2713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>45688</v>
       </c>
@@ -2733,7 +2738,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>45689</v>
       </c>
@@ -2762,7 +2767,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>45689</v>
       </c>
@@ -2787,7 +2792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>45689</v>
       </c>
@@ -2812,7 +2817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>45689</v>
       </c>
@@ -2837,7 +2842,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>45689</v>
       </c>
@@ -2862,7 +2867,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>45690</v>
       </c>
@@ -2891,7 +2896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>45690</v>
       </c>
@@ -2916,7 +2921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="7">
         <v>45690</v>
       </c>
@@ -2941,7 +2946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>45690</v>
       </c>
@@ -2970,7 +2975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="7">
         <v>45691</v>
       </c>
@@ -2995,7 +3000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="7">
         <v>45691</v>
       </c>
@@ -3020,7 +3025,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="7">
         <v>45692</v>
       </c>
@@ -3043,7 +3048,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="7">
         <v>45692</v>
       </c>
@@ -3068,7 +3073,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="7">
         <v>45693</v>
       </c>
@@ -3093,7 +3098,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="7">
         <v>45693</v>
       </c>
@@ -3118,7 +3123,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="7">
         <v>45694</v>
       </c>
@@ -3143,7 +3148,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="7">
         <v>45695</v>
       </c>
@@ -3172,7 +3177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="7">
         <v>45695</v>
       </c>
@@ -3201,7 +3206,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="7">
         <v>45695</v>
       </c>
@@ -3230,7 +3235,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="7">
         <v>45695</v>
       </c>
@@ -3259,7 +3264,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="7">
         <v>45695</v>
       </c>
@@ -3284,7 +3289,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="7">
         <v>45696</v>
       </c>
@@ -3313,7 +3318,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="7">
         <v>45696</v>
       </c>
@@ -3342,7 +3347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="7">
         <v>45696</v>
       </c>
@@ -3371,7 +3376,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="7">
         <v>45696</v>
       </c>
@@ -3400,7 +3405,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="7">
         <v>45696</v>
       </c>
@@ -3429,7 +3434,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="7">
         <v>45696</v>
       </c>
@@ -3458,7 +3463,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="7">
         <v>45697</v>
       </c>
@@ -3487,7 +3492,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="7">
         <v>45697</v>
       </c>
@@ -3516,7 +3521,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="7">
         <v>45697</v>
       </c>
@@ -3545,7 +3550,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="7">
         <v>45697</v>
       </c>
@@ -3574,7 +3579,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="7">
         <v>45698</v>
       </c>
@@ -3603,7 +3608,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="7">
         <v>45698</v>
       </c>
@@ -3628,7 +3633,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="7">
         <v>45698</v>
       </c>
@@ -3653,7 +3658,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="7">
         <v>45698</v>
       </c>
@@ -3678,7 +3683,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="7">
         <v>45698</v>
       </c>
@@ -3703,7 +3708,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="7">
         <v>45698</v>
       </c>
@@ -3728,7 +3733,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="7">
         <v>45699</v>
       </c>
@@ -3753,7 +3758,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="7">
         <v>45699</v>
       </c>
@@ -3778,7 +3783,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="7">
         <v>45699</v>
       </c>
@@ -3803,7 +3808,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="7">
         <v>45700</v>
       </c>
@@ -3828,7 +3833,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="7">
         <v>45700</v>
       </c>
@@ -3853,7 +3858,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="7">
         <v>45700</v>
       </c>
@@ -3878,7 +3883,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="7">
         <v>45700</v>
       </c>
@@ -3903,7 +3908,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="7">
         <v>45701</v>
       </c>
@@ -3932,7 +3937,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="7">
         <v>45701</v>
       </c>
@@ -3957,7 +3962,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="7">
         <v>45702</v>
       </c>
@@ -3982,7 +3987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="7">
         <v>45703</v>
       </c>
@@ -4007,7 +4012,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="7">
         <v>45703</v>
       </c>
@@ -4032,7 +4037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="7">
         <v>45703</v>
       </c>
@@ -4057,7 +4062,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="7">
         <v>45704</v>
       </c>
@@ -4082,7 +4087,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="7">
         <v>45704</v>
       </c>
@@ -4107,7 +4112,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="7">
         <v>45704</v>
       </c>
@@ -4132,7 +4137,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="7">
         <v>45704</v>
       </c>
@@ -4157,7 +4162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="7">
         <v>45704</v>
       </c>
@@ -4182,7 +4187,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="7">
         <v>45704</v>
       </c>
@@ -4207,7 +4212,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="7">
         <v>45704</v>
       </c>
@@ -4236,7 +4241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="7">
         <v>45705</v>
       </c>
@@ -4261,7 +4266,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="7">
         <v>45706</v>
       </c>
@@ -4286,7 +4291,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="7">
         <v>45707</v>
       </c>
@@ -4311,7 +4316,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="7">
         <v>45707</v>
       </c>
@@ -4340,7 +4345,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="7">
         <v>45708</v>
       </c>
@@ -4365,7 +4370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="7">
         <v>45708</v>
       </c>
@@ -4415,7 +4420,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="7">
         <v>45709</v>
       </c>
@@ -4440,7 +4445,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="7">
         <v>45709</v>
       </c>
@@ -4465,7 +4470,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="7">
         <v>45710</v>
       </c>
@@ -4494,7 +4499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="7">
         <v>45710</v>
       </c>
@@ -4519,7 +4524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="7">
         <v>45710</v>
       </c>
@@ -4544,7 +4549,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="7">
         <v>45710</v>
       </c>
@@ -4569,7 +4574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="7">
         <v>45710</v>
       </c>
@@ -4619,7 +4624,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="7">
         <v>45711</v>
       </c>
@@ -4644,7 +4649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="7">
         <v>45712</v>
       </c>
@@ -4652,24 +4657,24 @@
         <v>74</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D138" s="8"/>
       <c r="E138" s="8"/>
       <c r="F138" s="8" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="G138" s="9">
-        <v>45.91</v>
+        <v>11.27</v>
       </c>
       <c r="H138" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I138" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="7">
         <v>45712</v>
       </c>
@@ -4677,24 +4682,24 @@
         <v>74</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D139" s="8"/>
       <c r="E139" s="8"/>
       <c r="F139" s="8" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
       <c r="G139" s="9">
-        <v>11.27</v>
+        <v>3.85</v>
       </c>
       <c r="H139" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I139" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="7">
         <v>45712</v>
       </c>
@@ -4702,40 +4707,40 @@
         <v>74</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D140" s="8"/>
       <c r="E140" s="8"/>
       <c r="F140" s="8" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="G140" s="9">
-        <v>3.85</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H140" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I140" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="7">
-        <v>45712</v>
+        <v>45713</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>15</v>
+        <v>143</v>
       </c>
       <c r="D141" s="8"/>
       <c r="E141" s="8"/>
       <c r="F141" s="8" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="G141" s="9">
-        <v>9.3000000000000007</v>
+        <v>46.81</v>
       </c>
       <c r="H141" s="8" t="s">
         <v>10</v>
@@ -4744,7 +4749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="7">
         <v>45713</v>
       </c>
@@ -4752,15 +4757,15 @@
         <v>74</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
       <c r="F142" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G142" s="9">
-        <v>46.81</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="H142" s="8" t="s">
         <v>10</v>
@@ -4769,57 +4774,57 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="7">
-        <v>45713</v>
+        <v>45714</v>
       </c>
       <c r="B143" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D143" s="8"/>
       <c r="E143" s="8"/>
       <c r="F143" s="8" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="G143" s="9">
-        <v>4.8899999999999997</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H143" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I143" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="7">
-        <v>45714</v>
+        <v>45715</v>
       </c>
       <c r="B144" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D144" s="8"/>
       <c r="E144" s="8"/>
       <c r="F144" s="8" t="s">
-        <v>39</v>
+        <v>145</v>
       </c>
       <c r="G144" s="9">
-        <v>2.2999999999999998</v>
+        <v>14.3</v>
       </c>
       <c r="H144" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I144" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="7">
         <v>45715</v>
       </c>
@@ -4827,15 +4832,15 @@
         <v>74</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D145" s="8"/>
       <c r="E145" s="8"/>
       <c r="F145" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G145" s="9">
-        <v>14.3</v>
+        <v>10</v>
       </c>
       <c r="H145" s="8" t="s">
         <v>10</v>
@@ -4844,32 +4849,36 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="7">
-        <v>45715</v>
+        <v>45716</v>
       </c>
       <c r="B146" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D146" s="8"/>
-      <c r="E146" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="D146" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E146" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="F146" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G146" s="9">
-        <v>10</v>
+        <v>22.4</v>
       </c>
       <c r="H146" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I146" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="7">
         <v>45716</v>
       </c>
@@ -4883,13 +4892,13 @@
         <v>83</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="F147" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G147" s="9">
-        <v>22.4</v>
+        <v>8.6</v>
       </c>
       <c r="H147" s="8" t="s">
         <v>22</v>
@@ -4898,7 +4907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" s="7">
         <v>45716</v>
       </c>
@@ -4909,16 +4918,16 @@
         <v>29</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="E148" s="8" t="s">
         <v>129</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G148" s="9">
-        <v>8.6</v>
+        <v>6.5</v>
       </c>
       <c r="H148" s="8" t="s">
         <v>22</v>
@@ -4927,7 +4936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" s="7">
         <v>45716</v>
       </c>
@@ -4938,16 +4947,16 @@
         <v>29</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E149" s="8" t="s">
         <v>129</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G149" s="9">
-        <v>6.5</v>
+        <v>2.11</v>
       </c>
       <c r="H149" s="8" t="s">
         <v>22</v>
@@ -4956,7 +4965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" s="7">
         <v>45716</v>
       </c>
@@ -4967,16 +4976,16 @@
         <v>29</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="E150" s="8" t="s">
         <v>129</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G150" s="9">
-        <v>2.11</v>
+        <v>36.9</v>
       </c>
       <c r="H150" s="8" t="s">
         <v>22</v>
@@ -4985,7 +4994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="7">
         <v>45716</v>
       </c>
@@ -4996,16 +5005,16 @@
         <v>29</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E151" s="8" t="s">
         <v>129</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G151" s="9">
-        <v>36.9</v>
+        <v>9.1</v>
       </c>
       <c r="H151" s="8" t="s">
         <v>22</v>
@@ -5014,27 +5023,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="7">
-        <v>45716</v>
+        <v>45717</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C152" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="E152" s="8" t="s">
         <v>129</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G152" s="9">
-        <v>9.1</v>
+        <v>15.4</v>
       </c>
       <c r="H152" s="8" t="s">
         <v>22</v>
@@ -5043,7 +5052,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" s="7">
         <v>45717</v>
       </c>
@@ -5054,16 +5063,16 @@
         <v>29</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="E153" s="8" t="s">
         <v>129</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G153" s="9">
-        <v>15.4</v>
+        <v>7</v>
       </c>
       <c r="H153" s="8" t="s">
         <v>22</v>
@@ -5072,7 +5081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" s="7">
         <v>45717</v>
       </c>
@@ -5083,16 +5092,16 @@
         <v>29</v>
       </c>
       <c r="D154" s="8" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="E154" s="8" t="s">
         <v>129</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>154</v>
+        <v>39</v>
       </c>
       <c r="G154" s="9">
-        <v>7</v>
+        <v>5.9</v>
       </c>
       <c r="H154" s="8" t="s">
         <v>22</v>
@@ -5101,7 +5110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" s="7">
         <v>45717</v>
       </c>
@@ -5121,7 +5130,7 @@
         <v>39</v>
       </c>
       <c r="G155" s="9">
-        <v>5.9</v>
+        <v>5</v>
       </c>
       <c r="H155" s="8" t="s">
         <v>22</v>
@@ -5130,36 +5139,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" s="7">
-        <v>45717</v>
+        <v>45718</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D156" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E156" s="8" t="s">
-        <v>129</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D156" s="8"/>
+      <c r="E156" s="8"/>
       <c r="F156" s="8" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="G156" s="9">
-        <v>5</v>
+        <v>10.210000000000001</v>
       </c>
       <c r="H156" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I156" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" s="7">
         <v>45718</v>
       </c>
@@ -5172,10 +5177,10 @@
       <c r="D157" s="8"/>
       <c r="E157" s="8"/>
       <c r="F157" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G157" s="9">
-        <v>10.210000000000001</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="H157" s="8" t="s">
         <v>10</v>
@@ -5184,32 +5189,36 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" s="7">
-        <v>45718</v>
+        <v>45719</v>
       </c>
       <c r="B158" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D158" s="8"/>
-      <c r="E158" s="8"/>
-      <c r="F158" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G158" s="9">
-        <v>17.399999999999999</v>
+        <v>29</v>
+      </c>
+      <c r="D158" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E158" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F158" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G158" s="12">
+        <v>76.680000000000007</v>
       </c>
       <c r="H158" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I158" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" s="7">
         <v>45719</v>
       </c>
@@ -5217,53 +5226,53 @@
         <v>79</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D159" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E159" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="F159" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="G159" s="12">
-        <v>76.680000000000007</v>
+        <v>12</v>
+      </c>
+      <c r="D159" s="8"/>
+      <c r="E159" s="8"/>
+      <c r="F159" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G159" s="9">
+        <v>7.16</v>
       </c>
       <c r="H159" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I159" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="7">
-        <v>45719</v>
+        <v>45720</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D160" s="8"/>
-      <c r="E160" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="D160" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E160" s="8" t="s">
+        <v>159</v>
+      </c>
       <c r="F160" s="8" t="s">
-        <v>32</v>
+        <v>160</v>
       </c>
       <c r="G160" s="9">
-        <v>7.16</v>
+        <v>6.2</v>
       </c>
       <c r="H160" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I160" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" s="7">
         <v>45720</v>
       </c>
@@ -5274,16 +5283,16 @@
         <v>29</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>159</v>
       </c>
       <c r="F161" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G161" s="9">
-        <v>6.2</v>
+        <v>41.2</v>
       </c>
       <c r="H161" s="8" t="s">
         <v>22</v>
@@ -5292,9 +5301,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" s="7">
-        <v>45720</v>
+        <v>45721</v>
       </c>
       <c r="B162" s="8" t="s">
         <v>79</v>
@@ -5303,16 +5312,16 @@
         <v>29</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="E162" s="8" t="s">
         <v>159</v>
       </c>
       <c r="F162" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G162" s="9">
-        <v>41.2</v>
+        <v>18.75</v>
       </c>
       <c r="H162" s="8" t="s">
         <v>22</v>
@@ -5321,7 +5330,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" s="7">
         <v>45721</v>
       </c>
@@ -5329,28 +5338,24 @@
         <v>79</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D163" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E163" s="8" t="s">
-        <v>159</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D163" s="8"/>
+      <c r="E163" s="8"/>
       <c r="F163" s="8" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="G163" s="9">
-        <v>18.75</v>
+        <v>2.5</v>
       </c>
       <c r="H163" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I163" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="7">
         <v>45721</v>
       </c>
@@ -5363,10 +5368,10 @@
       <c r="D164" s="8"/>
       <c r="E164" s="8"/>
       <c r="F164" s="8" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="G164" s="9">
-        <v>2.5</v>
+        <v>7.68</v>
       </c>
       <c r="H164" s="8" t="s">
         <v>10</v>
@@ -5375,32 +5380,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" s="7">
-        <v>45721</v>
+        <v>45722</v>
       </c>
       <c r="B165" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D165" s="8"/>
       <c r="E165" s="8"/>
       <c r="F165" s="8" t="s">
-        <v>59</v>
+        <v>163</v>
       </c>
       <c r="G165" s="9">
-        <v>7.68</v>
+        <v>17.649999999999999</v>
       </c>
       <c r="H165" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I165" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="7">
         <v>45722</v>
       </c>
@@ -5408,24 +5413,24 @@
         <v>79</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D166" s="8"/>
       <c r="E166" s="8"/>
       <c r="F166" s="8" t="s">
-        <v>163</v>
+        <v>59</v>
       </c>
       <c r="G166" s="9">
-        <v>17.649999999999999</v>
+        <v>29.12</v>
       </c>
       <c r="H166" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I166" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" s="7">
         <v>45722</v>
       </c>
@@ -5438,10 +5443,10 @@
       <c r="D167" s="8"/>
       <c r="E167" s="8"/>
       <c r="F167" s="8" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="G167" s="9">
-        <v>29.12</v>
+        <v>5</v>
       </c>
       <c r="H167" s="8" t="s">
         <v>10</v>
@@ -5450,32 +5455,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="7">
-        <v>45722</v>
+        <v>45723</v>
       </c>
       <c r="B168" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D168" s="8"/>
       <c r="E168" s="8"/>
       <c r="F168" s="8" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="G168" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H168" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I168" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" s="7">
         <v>45723</v>
       </c>
@@ -5483,49 +5488,53 @@
         <v>79</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D169" s="8"/>
       <c r="E169" s="8"/>
       <c r="F169" s="8" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="G169" s="9">
-        <v>6</v>
+        <v>12.16</v>
       </c>
       <c r="H169" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I169" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" s="7">
-        <v>45723</v>
+        <v>45724</v>
       </c>
       <c r="B170" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C170" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D170" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D170" s="8"/>
-      <c r="E170" s="8"/>
+      <c r="E170" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="F170" s="8" t="s">
         <v>155</v>
       </c>
       <c r="G170" s="9">
-        <v>12.16</v>
+        <v>11.11</v>
       </c>
       <c r="H170" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I170" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" s="7">
         <v>45724</v>
       </c>
@@ -5536,16 +5545,16 @@
         <v>29</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="E171" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="G171" s="9">
-        <v>11.11</v>
+        <v>28</v>
       </c>
       <c r="H171" s="8" t="s">
         <v>22</v>
@@ -5554,7 +5563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="7">
         <v>45724</v>
       </c>
@@ -5565,16 +5574,16 @@
         <v>29</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>165</v>
+        <v>28</v>
       </c>
       <c r="G172" s="9">
-        <v>28</v>
+        <v>1.2</v>
       </c>
       <c r="H172" s="8" t="s">
         <v>22</v>
@@ -5583,7 +5592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" s="7">
         <v>45724</v>
       </c>
@@ -5594,25 +5603,25 @@
         <v>29</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E173" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>28</v>
+        <v>166</v>
       </c>
       <c r="G173" s="9">
-        <v>1.2</v>
+        <v>12</v>
       </c>
       <c r="H173" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I173" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="7">
         <v>45724</v>
       </c>
@@ -5629,10 +5638,10 @@
         <v>94</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G174" s="9">
-        <v>12</v>
+        <v>4.5</v>
       </c>
       <c r="H174" s="8" t="s">
         <v>10</v>
@@ -5641,7 +5650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" s="7">
         <v>45724</v>
       </c>
@@ -5652,27 +5661,27 @@
         <v>29</v>
       </c>
       <c r="D175" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E175" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G175" s="9">
-        <v>4.5</v>
+        <v>11</v>
       </c>
       <c r="H175" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I175" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="7">
-        <v>45724</v>
+        <v>45725</v>
       </c>
       <c r="B176" s="8" t="s">
         <v>79</v>
@@ -5681,25 +5690,25 @@
         <v>29</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E176" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="G176" s="9">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H176" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I176" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" s="7">
         <v>45725</v>
       </c>
@@ -5710,25 +5719,25 @@
         <v>29</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E177" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>39</v>
+        <v>168</v>
       </c>
       <c r="G177" s="9">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H177" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I177" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="7">
         <v>45725</v>
       </c>
@@ -5739,16 +5748,16 @@
         <v>29</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E178" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F178" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G178" s="9">
-        <v>15</v>
+        <v>19.5</v>
       </c>
       <c r="H178" s="8" t="s">
         <v>22</v>
@@ -5757,7 +5766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="7">
         <v>45725</v>
       </c>
@@ -5768,16 +5777,16 @@
         <v>29</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="E179" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G179" s="9">
-        <v>19.5</v>
+        <v>18</v>
       </c>
       <c r="H179" s="8" t="s">
         <v>22</v>
@@ -5786,7 +5795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="7">
         <v>45725</v>
       </c>
@@ -5797,16 +5806,16 @@
         <v>29</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G180" s="9">
-        <v>18</v>
+        <v>12.5</v>
       </c>
       <c r="H180" s="8" t="s">
         <v>22</v>
@@ -5815,7 +5824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" s="7">
         <v>45725</v>
       </c>
@@ -5832,10 +5841,10 @@
         <v>94</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="G181" s="9">
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="H181" s="8" t="s">
         <v>22</v>
@@ -5844,9 +5853,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="7">
-        <v>45725</v>
+        <v>45726</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>79</v>
@@ -5855,16 +5864,16 @@
         <v>29</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="E182" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="G182" s="9">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H182" s="8" t="s">
         <v>22</v>
@@ -5873,7 +5882,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="7">
         <v>45726</v>
       </c>
@@ -5884,16 +5893,16 @@
         <v>29</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="E183" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G183" s="9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H183" s="8" t="s">
         <v>22</v>
@@ -5902,7 +5911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="7">
         <v>45726</v>
       </c>
@@ -5919,19 +5928,19 @@
         <v>94</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G184" s="9">
-        <v>5</v>
+        <v>13.5</v>
       </c>
       <c r="H184" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I184" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="7">
         <v>45726</v>
       </c>
@@ -5948,19 +5957,19 @@
         <v>94</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G185" s="9">
-        <v>13.5</v>
+        <v>3</v>
       </c>
       <c r="H185" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I185" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="7">
         <v>45726</v>
       </c>
@@ -5977,10 +5986,10 @@
         <v>94</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="G186" s="9">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="H186" s="8" t="s">
         <v>22</v>
@@ -5989,9 +5998,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="7">
-        <v>45726</v>
+        <v>45727</v>
       </c>
       <c r="B187" s="8" t="s">
         <v>79</v>
@@ -6000,25 +6009,25 @@
         <v>29</v>
       </c>
       <c r="D187" s="8" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E187" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G187" s="9">
-        <v>17</v>
+        <v>5.2</v>
       </c>
       <c r="H187" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I187" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" s="7">
         <v>45727</v>
       </c>
@@ -6029,16 +6038,16 @@
         <v>29</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="E188" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G188" s="9">
-        <v>5.2</v>
+        <v>10</v>
       </c>
       <c r="H188" s="8" t="s">
         <v>10</v>
@@ -6047,7 +6056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="7">
         <v>45727</v>
       </c>
@@ -6058,16 +6067,16 @@
         <v>29</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="E189" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G189" s="9">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H189" s="8" t="s">
         <v>10</v>
@@ -6076,7 +6085,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" s="7">
         <v>45727</v>
       </c>
@@ -6087,25 +6096,25 @@
         <v>29</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E190" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G190" s="9">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="H190" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I190" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" s="7">
         <v>45727</v>
       </c>
@@ -6116,16 +6125,16 @@
         <v>29</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E191" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F191" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G191" s="9">
-        <v>1.5</v>
+        <v>21</v>
       </c>
       <c r="H191" s="8" t="s">
         <v>22</v>
@@ -6134,7 +6143,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" s="7">
         <v>45727</v>
       </c>
@@ -6151,10 +6160,10 @@
         <v>94</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G192" s="9">
-        <v>21</v>
+        <v>2.75</v>
       </c>
       <c r="H192" s="8" t="s">
         <v>22</v>
@@ -6163,7 +6172,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" s="7">
         <v>45727</v>
       </c>
@@ -6174,16 +6183,16 @@
         <v>29</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>180</v>
+        <v>39</v>
       </c>
       <c r="G193" s="9">
-        <v>2.75</v>
+        <v>4.5</v>
       </c>
       <c r="H193" s="8" t="s">
         <v>22</v>
@@ -6192,27 +6201,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" s="7">
-        <v>45727</v>
+        <v>45728</v>
       </c>
       <c r="B194" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D194" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E194" s="8" t="s">
-        <v>94</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D194" s="8"/>
+      <c r="E194" s="8"/>
       <c r="F194" s="8" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="G194" s="9">
-        <v>4.5</v>
+        <v>12.26</v>
       </c>
       <c r="H194" s="8" t="s">
         <v>22</v>
@@ -6221,7 +6226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" s="7">
         <v>45728</v>
       </c>
@@ -6229,49 +6234,53 @@
         <v>79</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D195" s="8"/>
       <c r="E195" s="8"/>
       <c r="F195" s="8" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="G195" s="9">
-        <v>12.26</v>
+        <v>31.66</v>
       </c>
       <c r="H195" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I195" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" s="7">
-        <v>45728</v>
+        <v>45729</v>
       </c>
       <c r="B196" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D196" s="8"/>
-      <c r="E196" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="D196" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E196" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="F196" s="8" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="G196" s="9">
-        <v>31.66</v>
+        <v>9.65</v>
       </c>
       <c r="H196" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I196" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" s="7">
         <v>45729</v>
       </c>
@@ -6282,16 +6291,16 @@
         <v>29</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G197" s="9">
-        <v>9.65</v>
+        <v>1.5</v>
       </c>
       <c r="H197" s="8" t="s">
         <v>22</v>
@@ -6300,36 +6309,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" s="7">
-        <v>45729</v>
+        <v>45730</v>
       </c>
       <c r="B198" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D198" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E198" s="8" t="s">
-        <v>94</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D198" s="8"/>
+      <c r="E198" s="8"/>
       <c r="F198" s="8" t="s">
-        <v>182</v>
+        <v>59</v>
       </c>
       <c r="G198" s="9">
-        <v>1.5</v>
+        <v>17.52</v>
       </c>
       <c r="H198" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I198" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" s="7">
         <v>45730</v>
       </c>
@@ -6342,10 +6347,10 @@
       <c r="D199" s="8"/>
       <c r="E199" s="8"/>
       <c r="F199" s="8" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="G199" s="9">
-        <v>17.52</v>
+        <v>6.14</v>
       </c>
       <c r="H199" s="8" t="s">
         <v>10</v>
@@ -6354,32 +6359,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" s="7">
-        <v>45730</v>
+        <v>45731</v>
       </c>
       <c r="B200" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C200" s="8" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D200" s="8"/>
       <c r="E200" s="8"/>
       <c r="F200" s="8" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="G200" s="9">
-        <v>6.14</v>
+        <v>35</v>
       </c>
       <c r="H200" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I200" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" s="7">
         <v>45731</v>
       </c>
@@ -6387,40 +6392,40 @@
         <v>79</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D201" s="8"/>
       <c r="E201" s="8"/>
       <c r="F201" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G201" s="9">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="H201" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I201" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" s="7">
-        <v>45731</v>
+        <v>45732</v>
       </c>
       <c r="B202" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C202" s="8" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D202" s="8"/>
       <c r="E202" s="8"/>
       <c r="F202" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G202" s="9">
-        <v>8</v>
+        <v>22.2</v>
       </c>
       <c r="H202" s="8" t="s">
         <v>10</v>
@@ -6429,7 +6434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" s="7">
         <v>45732</v>
       </c>
@@ -6442,10 +6447,10 @@
       <c r="D203" s="8"/>
       <c r="E203" s="8"/>
       <c r="F203" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G203" s="9">
-        <v>22.2</v>
+        <v>61.25</v>
       </c>
       <c r="H203" s="8" t="s">
         <v>10</v>
@@ -6454,7 +6459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" s="7">
         <v>45732</v>
       </c>
@@ -6467,19 +6472,19 @@
       <c r="D204" s="8"/>
       <c r="E204" s="8"/>
       <c r="F204" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G204" s="9">
-        <v>61.25</v>
+        <v>59.99</v>
       </c>
       <c r="H204" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I204" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" s="7">
         <v>45732</v>
       </c>
@@ -6492,10 +6497,10 @@
       <c r="D205" s="8"/>
       <c r="E205" s="8"/>
       <c r="F205" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G205" s="9">
-        <v>59.99</v>
+        <v>70.599999999999994</v>
       </c>
       <c r="H205" s="8" t="s">
         <v>22</v>
@@ -6504,7 +6509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" s="7">
         <v>45732</v>
       </c>
@@ -6512,15 +6517,15 @@
         <v>79</v>
       </c>
       <c r="C206" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D206" s="8"/>
       <c r="E206" s="8"/>
       <c r="F206" s="8" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="G206" s="9">
-        <v>70.599999999999994</v>
+        <v>16.059999999999999</v>
       </c>
       <c r="H206" s="8" t="s">
         <v>22</v>
@@ -6529,57 +6534,57 @@
         <v>11</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" s="7">
-        <v>45732</v>
+        <v>45733</v>
       </c>
       <c r="B207" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C207" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D207" s="8"/>
       <c r="E207" s="8"/>
       <c r="F207" s="8" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="G207" s="9">
-        <v>16.059999999999999</v>
+        <v>27.61</v>
       </c>
       <c r="H207" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I207" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" s="7">
-        <v>45733</v>
+        <v>45735</v>
       </c>
       <c r="B208" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D208" s="8"/>
       <c r="E208" s="8"/>
       <c r="F208" s="8" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
       <c r="G208" s="9">
-        <v>27.61</v>
+        <v>25.8</v>
       </c>
       <c r="H208" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I208" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" s="7">
         <v>45735</v>
       </c>
@@ -6592,44 +6597,48 @@
       <c r="D209" s="8"/>
       <c r="E209" s="8"/>
       <c r="F209" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G209" s="9">
-        <v>25.8</v>
+        <v>11.9</v>
       </c>
       <c r="H209" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I209" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" s="7">
-        <v>45735</v>
+        <v>45736</v>
       </c>
       <c r="B210" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D210" s="8"/>
-      <c r="E210" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="D210" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E210" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="F210" s="8" t="s">
-        <v>190</v>
+        <v>39</v>
       </c>
       <c r="G210" s="9">
-        <v>11.9</v>
+        <v>6.9</v>
       </c>
       <c r="H210" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I210" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" s="7">
         <v>45736</v>
       </c>
@@ -6640,16 +6649,16 @@
         <v>29</v>
       </c>
       <c r="D211" s="8" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E211" s="8" t="s">
         <v>157</v>
       </c>
       <c r="F211" s="8" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
       <c r="G211" s="9">
-        <v>6.9</v>
+        <v>29</v>
       </c>
       <c r="H211" s="8" t="s">
         <v>22</v>
@@ -6658,7 +6667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" s="7">
         <v>45736</v>
       </c>
@@ -6669,16 +6678,16 @@
         <v>29</v>
       </c>
       <c r="D212" s="8" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E212" s="8" t="s">
         <v>157</v>
       </c>
       <c r="F212" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G212" s="9">
-        <v>29</v>
+        <v>8.9</v>
       </c>
       <c r="H212" s="8" t="s">
         <v>22</v>
@@ -6687,9 +6696,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" s="7">
-        <v>45736</v>
+        <v>45737</v>
       </c>
       <c r="B213" s="8" t="s">
         <v>79</v>
@@ -6704,10 +6713,10 @@
         <v>157</v>
       </c>
       <c r="F213" s="8" t="s">
-        <v>192</v>
+        <v>39</v>
       </c>
       <c r="G213" s="9">
-        <v>8.9</v>
+        <v>9</v>
       </c>
       <c r="H213" s="8" t="s">
         <v>22</v>
@@ -6716,7 +6725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" s="7">
         <v>45737</v>
       </c>
@@ -6727,16 +6736,16 @@
         <v>29</v>
       </c>
       <c r="D214" s="8" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="E214" s="8" t="s">
         <v>157</v>
       </c>
       <c r="F214" s="8" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G214" s="9">
-        <v>9</v>
+        <v>12.25</v>
       </c>
       <c r="H214" s="8" t="s">
         <v>22</v>
@@ -6745,9 +6754,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" s="7">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B215" s="8" t="s">
         <v>79</v>
@@ -6756,16 +6765,16 @@
         <v>29</v>
       </c>
       <c r="D215" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E215" s="8" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="F215" s="8" t="s">
-        <v>12</v>
+        <v>155</v>
       </c>
       <c r="G215" s="9">
-        <v>12.25</v>
+        <v>6.8</v>
       </c>
       <c r="H215" s="8" t="s">
         <v>22</v>
@@ -6774,7 +6783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" s="7">
         <v>45738</v>
       </c>
@@ -6782,19 +6791,15 @@
         <v>79</v>
       </c>
       <c r="C216" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D216" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E216" s="8" t="s">
-        <v>193</v>
-      </c>
+      <c r="D216" s="8"/>
+      <c r="E216" s="8"/>
       <c r="F216" s="8" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="G216" s="9">
-        <v>6.8</v>
+        <v>7.99</v>
       </c>
       <c r="H216" s="8" t="s">
         <v>22</v>
@@ -6803,57 +6808,61 @@
         <v>11</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" s="7">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B217" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C217" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D217" s="8"/>
       <c r="E217" s="8"/>
       <c r="F217" s="8" t="s">
-        <v>194</v>
+        <v>146</v>
       </c>
       <c r="G217" s="9">
-        <v>7.99</v>
+        <v>10</v>
       </c>
       <c r="H217" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I217" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" s="7">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B218" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C218" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D218" s="8"/>
-      <c r="E218" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="D218" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E218" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="F218" s="8" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="G218" s="9">
-        <v>10</v>
+        <v>9.1</v>
       </c>
       <c r="H218" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I218" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" s="7">
         <v>45740</v>
       </c>
@@ -6864,16 +6873,16 @@
         <v>29</v>
       </c>
       <c r="D219" s="8" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="E219" s="8" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="F219" s="8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G219" s="9">
-        <v>9.1</v>
+        <v>18.2</v>
       </c>
       <c r="H219" s="8" t="s">
         <v>22</v>
@@ -6882,52 +6891,48 @@
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" s="7">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B220" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C220" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D220" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E220" s="8" t="s">
-        <v>193</v>
-      </c>
+      <c r="D220" s="8"/>
+      <c r="E220" s="8"/>
       <c r="F220" s="8" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="G220" s="9">
-        <v>18.2</v>
+        <v>25.62</v>
       </c>
       <c r="H220" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I220" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" s="7">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B221" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="D221" s="8"/>
       <c r="E221" s="8"/>
       <c r="F221" s="8" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="G221" s="9">
-        <v>25.62</v>
+        <v>3.99</v>
       </c>
       <c r="H221" s="8" t="s">
         <v>10</v>
@@ -6936,7 +6941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" s="7">
         <v>45742</v>
       </c>
@@ -6944,15 +6949,15 @@
         <v>79</v>
       </c>
       <c r="C222" s="8" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="D222" s="8"/>
       <c r="E222" s="8"/>
       <c r="F222" s="8" t="s">
-        <v>197</v>
+        <v>12</v>
       </c>
       <c r="G222" s="9">
-        <v>3.99</v>
+        <v>13.05</v>
       </c>
       <c r="H222" s="8" t="s">
         <v>10</v>
@@ -6961,23 +6966,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" s="7">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B223" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C223" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D223" s="8"/>
       <c r="E223" s="8"/>
       <c r="F223" s="8" t="s">
-        <v>12</v>
+        <v>198</v>
       </c>
       <c r="G223" s="9">
-        <v>13.05</v>
+        <v>5.9</v>
       </c>
       <c r="H223" s="8" t="s">
         <v>10</v>
@@ -6986,7 +6991,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" s="7">
         <v>45743</v>
       </c>
@@ -6994,15 +6999,15 @@
         <v>79</v>
       </c>
       <c r="C224" s="8" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D224" s="8"/>
       <c r="E224" s="8"/>
       <c r="F224" s="8" t="s">
-        <v>198</v>
+        <v>138</v>
       </c>
       <c r="G224" s="9">
-        <v>5.9</v>
+        <v>7.15</v>
       </c>
       <c r="H224" s="8" t="s">
         <v>10</v>
@@ -7011,9 +7016,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" s="7">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B225" s="8" t="s">
         <v>79</v>
@@ -7024,10 +7029,10 @@
       <c r="D225" s="8"/>
       <c r="E225" s="8"/>
       <c r="F225" s="8" t="s">
-        <v>138</v>
+        <v>39</v>
       </c>
       <c r="G225" s="9">
-        <v>7.15</v>
+        <v>5.3</v>
       </c>
       <c r="H225" s="8" t="s">
         <v>10</v>
@@ -7036,9 +7041,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" s="7">
-        <v>45744</v>
+        <v>45746</v>
       </c>
       <c r="B226" s="8" t="s">
         <v>79</v>
@@ -7052,7 +7057,7 @@
         <v>39</v>
       </c>
       <c r="G226" s="9">
-        <v>5.3</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="H226" s="8" t="s">
         <v>10</v>
@@ -7061,23 +7066,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" s="7">
-        <v>45746</v>
+        <v>45747</v>
       </c>
       <c r="B227" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C227" s="8" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D227" s="8"/>
       <c r="E227" s="8"/>
       <c r="F227" s="8" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="G227" s="9">
-        <v>4.8499999999999996</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="H227" s="8" t="s">
         <v>10</v>
@@ -7086,7 +7091,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" s="7">
         <v>45747</v>
       </c>
@@ -7094,24 +7099,28 @@
         <v>79</v>
       </c>
       <c r="C228" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D228" s="8"/>
-      <c r="E228" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="D228" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E228" s="8" t="s">
+        <v>200</v>
+      </c>
       <c r="F228" s="8" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
       <c r="G228" s="9">
-        <v>17.399999999999999</v>
+        <v>109.6</v>
       </c>
       <c r="H228" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I228" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" s="7">
         <v>45747</v>
       </c>
@@ -7119,44 +7128,40 @@
         <v>79</v>
       </c>
       <c r="C229" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D229" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E229" s="8" t="s">
-        <v>200</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D229" s="8"/>
+      <c r="E229" s="8"/>
       <c r="F229" s="8" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G229" s="9">
-        <v>109.6</v>
+        <v>22.4</v>
       </c>
       <c r="H229" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I229" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" s="7">
-        <v>45747</v>
+        <v>45748</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>79</v>
+        <v>207</v>
       </c>
       <c r="C230" s="8" t="s">
-        <v>15</v>
+        <v>143</v>
       </c>
       <c r="D230" s="8"/>
       <c r="E230" s="8"/>
       <c r="F230" s="8" t="s">
-        <v>201</v>
+        <v>143</v>
       </c>
       <c r="G230" s="9">
-        <v>22.4</v>
+        <v>34.520000000000003</v>
       </c>
       <c r="H230" s="8" t="s">
         <v>10</v>
@@ -7165,7 +7170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" s="7">
         <v>45748</v>
       </c>
@@ -7173,15 +7178,15 @@
         <v>207</v>
       </c>
       <c r="C231" s="8" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="D231" s="8"/>
       <c r="E231" s="8"/>
       <c r="F231" s="8" t="s">
-        <v>143</v>
+        <v>202</v>
       </c>
       <c r="G231" s="9">
-        <v>34.520000000000003</v>
+        <v>3.85</v>
       </c>
       <c r="H231" s="8" t="s">
         <v>10</v>
@@ -7190,7 +7195,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" s="7">
         <v>45748</v>
       </c>
@@ -7198,15 +7203,15 @@
         <v>207</v>
       </c>
       <c r="C232" s="8" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="D232" s="8"/>
       <c r="E232" s="8"/>
       <c r="F232" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G232" s="9">
-        <v>3.85</v>
+        <v>44</v>
       </c>
       <c r="H232" s="8" t="s">
         <v>10</v>
@@ -7215,7 +7220,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" s="7">
         <v>45748</v>
       </c>
@@ -7223,15 +7228,15 @@
         <v>207</v>
       </c>
       <c r="C233" s="8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D233" s="8"/>
       <c r="E233" s="8"/>
       <c r="F233" s="8" t="s">
-        <v>203</v>
+        <v>59</v>
       </c>
       <c r="G233" s="9">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H233" s="8" t="s">
         <v>10</v>
@@ -7240,7 +7245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" s="7">
         <v>45748</v>
       </c>
@@ -7248,15 +7253,15 @@
         <v>207</v>
       </c>
       <c r="C234" s="8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D234" s="8"/>
       <c r="E234" s="8"/>
       <c r="F234" s="8" t="s">
-        <v>59</v>
+        <v>204</v>
       </c>
       <c r="G234" s="9">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="H234" s="8" t="s">
         <v>10</v>
@@ -7265,9 +7270,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" s="7">
-        <v>45748</v>
+        <v>45749</v>
       </c>
       <c r="B235" s="8" t="s">
         <v>207</v>
@@ -7278,19 +7283,19 @@
       <c r="D235" s="8"/>
       <c r="E235" s="8"/>
       <c r="F235" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G235" s="9">
-        <v>10</v>
+        <v>7.5</v>
       </c>
       <c r="H235" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I235" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" s="7">
         <v>45749</v>
       </c>
@@ -7298,15 +7303,19 @@
         <v>207</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D236" s="8"/>
-      <c r="E236" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="D236" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E236" s="8" t="s">
+        <v>200</v>
+      </c>
       <c r="F236" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G236" s="9">
-        <v>7.5</v>
+        <v>16.48</v>
       </c>
       <c r="H236" s="8" t="s">
         <v>22</v>
@@ -7315,7 +7324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" s="7">
         <v>45749</v>
       </c>
@@ -7323,19 +7332,15 @@
         <v>207</v>
       </c>
       <c r="C237" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D237" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E237" s="8" t="s">
-        <v>200</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D237" s="8"/>
+      <c r="E237" s="8"/>
       <c r="F237" s="8" t="s">
-        <v>206</v>
+        <v>27</v>
       </c>
       <c r="G237" s="9">
-        <v>16.48</v>
+        <v>4.2</v>
       </c>
       <c r="H237" s="8" t="s">
         <v>22</v>
@@ -7345,29 +7350,15 @@
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A238" s="7">
-        <v>45749</v>
-      </c>
-      <c r="B238" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C238" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="A238" s="8"/>
+      <c r="B238" s="8"/>
+      <c r="C238" s="8"/>
       <c r="D238" s="8"/>
       <c r="E238" s="8"/>
-      <c r="F238" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G238" s="9">
-        <v>4.2</v>
-      </c>
-      <c r="H238" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I238" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="F238" s="8"/>
+      <c r="G238" s="9"/>
+      <c r="H238" s="8"/>
+      <c r="I238" s="8"/>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239" s="8"/>
@@ -11846,38 +11837,33 @@
       <c r="H645" s="8"/>
       <c r="I645" s="8"/>
     </row>
-    <row r="646" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A646" s="8"/>
-      <c r="B646" s="8"/>
-      <c r="C646" s="8"/>
-      <c r="D646" s="8"/>
-      <c r="E646" s="8"/>
-      <c r="F646" s="8"/>
-      <c r="G646" s="9"/>
-      <c r="H646" s="8"/>
-      <c r="I646" s="8"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I238" xr:uid="{73D03841-840F-48EF-840B-36FDA2E59E7D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I176">
-    <sortCondition ref="A109:A176"/>
+  <autoFilter ref="A1:I237" xr:uid="{73D03841-840F-48EF-840B-36FDA2E59E7D}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="CC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I175">
+    <sortCondition ref="A109:A175"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{790B5306-A74C-4E52-BB85-C4249CF769EB}">
+          <x14:formula1>
+            <xm:f>lists!$C$1:$C$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D13</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77508706-FF64-4936-A3A6-4F0639AF6AF4}">
           <x14:formula1>
             <xm:f>lists!$A$1:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{790B5306-A74C-4E52-BB85-C4249CF769EB}">
-          <x14:formula1>
-            <xm:f>lists!$C$1:$C$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E87165FA-15D3-4B9C-BFC7-CBABAFD0C4D5}">
           <x14:formula1>

</xml_diff>